<commit_message>
[Change] Reformat Peer Review
</commit_message>
<xml_diff>
--- a/Design Docs/PeerReview.xlsx
+++ b/Design Docs/PeerReview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project-startup\Design Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37601BAE-D686-4D09-98F0-4DE674B37ABA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7D2D9F-950F-4251-AB38-DE6C4BFC0111}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="53">
   <si>
     <t>PEER1</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t xml:space="preserve">everyone enjoys my additude, but I should stay realistic and focussed. </t>
+  </si>
+  <si>
+    <t>Rob O'Connor</t>
   </si>
 </sst>
 </file>
@@ -1119,7 +1122,7 @@
   <dimension ref="A1:Z18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1361,7 +1364,7 @@
       </c>
       <c r="D6" s="18" t="str">
         <f>CONCATENATE("Review of ",C7)</f>
-        <v>Review of Team Member 1</v>
+        <v>Review of Rob O'Connor</v>
       </c>
       <c r="E6" s="19" t="s">
         <v>23</v>
@@ -1442,10 +1445,10 @@
         <v>26</v>
       </c>
       <c r="B7" s="20">
-        <v>13335</v>
+        <v>445921</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="D7" s="22" t="s">
         <v>28</v>
@@ -4227,7 +4230,7 @@
       <c r="A1" s="34"/>
       <c r="B1" s="36" t="str">
         <f>'Week 2 Review'!C7</f>
-        <v>Team Member 1</v>
+        <v>Rob O'Connor</v>
       </c>
       <c r="E1" s="34"/>
       <c r="F1" s="36" t="str">

</xml_diff>

<commit_message>
[ADD] My peer review
</commit_message>
<xml_diff>
--- a/Design Docs/PeerReview.xlsx
+++ b/Design Docs/PeerReview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project-startup\Design Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDB8D60-05F9-420E-92FA-0E06EC3D55B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52F26A3-6298-46A4-B58C-6C399DB7F1F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="60">
   <si>
     <t>PEER1</t>
   </si>
@@ -203,8 +203,48 @@
   </si>
   <si>
     <t xml:space="preserve">Strength(s):
-Punctuality Improved compared previous Projects.
-Improvement(s):
+Punctuality Improved compared previous Projects, planning
+for Arti and Design pretty acccurate, Kept meeting flowing wee
+Improvement(s): More Art work done, Went too traditonal with
+the marketing plan, need to try and do financials by myself
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strength(s): Finished all work on time, high quality 2D art,
+good contrbution during team discussion (Liked the idea
+you pitched about space)  Strikes the correct balance fun/professioinalism
+Improvement(s): Take more confidnece in your descisions
+you're normally right when it comes to your tasks
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strength(s): Reacting well to being lead of other programmers, knowledge of engine programming 
+helping the project along, good communication
+Improvement(s): At times gets stuck on tiny details when
+discussing things, is a benefit at times but sometimes it
+slows progress a bit
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strength(s): Great Communication, Not afraid to just sit 
+and learn how to do something,, never rejects tasks
+Improvement(s): Punctuality could be better
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strength(s):  All work finished on time, dived in to topics
+not of his expertise (Level Design and to lesser extent
+concept art) Produced really nice concept for music
+very quickly, Strikes the correct balance fun/professioinalism
+Improvement(s): at times communication coould be better
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strength(s): Madre the initial prototyoe very quicjly
+and never says no to adding a new feature, adds 
+logiical feedback when talking about dsign
+Improvement(s): Sometimes get stuck onj points
+during discussions
 </t>
   </si>
 </sst>
@@ -1130,8 +1170,8 @@
   </sheetPr>
   <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="G4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1462,27 +1502,39 @@
       <c r="D7" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="42"/>
+      <c r="E7" s="42">
+        <v>7</v>
+      </c>
       <c r="F7" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="42"/>
+        <v>55</v>
+      </c>
+      <c r="G7" s="42">
+        <v>8</v>
+      </c>
       <c r="H7" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" s="42"/>
+        <v>58</v>
+      </c>
+      <c r="I7" s="42">
+        <v>8</v>
+      </c>
       <c r="J7" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="K7" s="42"/>
+        <v>59</v>
+      </c>
+      <c r="K7" s="42">
+        <v>8</v>
+      </c>
       <c r="L7" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="M7" s="24"/>
+        <v>56</v>
+      </c>
+      <c r="M7" s="24">
+        <v>8</v>
+      </c>
       <c r="N7" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="O7" s="24"/>
+        <v>57</v>
+      </c>
+      <c r="O7" s="24">
+        <v>7</v>
+      </c>
       <c r="P7" s="22" t="s">
         <v>28</v>
       </c>
@@ -1978,44 +2030,44 @@
       <c r="D17" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="33" t="str">
+      <c r="E17" s="33">
         <f>IF(COUNTA(E7:E16)&gt;0,COUNT(E7:E16)/COUNTA(E7:E16),"NA")</f>
-        <v>NA</v>
+        <v>1</v>
       </c>
       <c r="F17" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="33" t="str">
+      <c r="G17" s="33">
         <f>IF(COUNTA(G7:G16)&gt;0,COUNT(G7:G16)/COUNTA(G7:G16),"NA")</f>
-        <v>NA</v>
+        <v>1</v>
       </c>
       <c r="H17" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="I17" s="33" t="str">
+      <c r="I17" s="33">
         <f>IF(COUNTA(I7:I16)&gt;0,COUNT(I7:I16)/COUNTA(I7:I16),"NA")</f>
-        <v>NA</v>
+        <v>1</v>
       </c>
       <c r="J17" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="K17" s="33" t="str">
+      <c r="K17" s="33">
         <f>IF(COUNTA(K7:K16)&gt;0,COUNT(K7:K16)/COUNTA(K7:K16),"NA")</f>
-        <v>NA</v>
+        <v>1</v>
       </c>
       <c r="L17" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="M17" s="33" t="str">
+      <c r="M17" s="33">
         <f>IF(COUNTA(M7:M16)&gt;0,COUNT(M7:M16)/COUNTA(M7:M16),"NA")</f>
-        <v>NA</v>
+        <v>1</v>
       </c>
       <c r="N17" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="O17" s="33" t="str">
+      <c r="O17" s="33">
         <f>IF(COUNTA(O7:O16)&gt;0,COUNT(O7:O16)/COUNTA(O7:O16),"NA")</f>
-        <v>NA</v>
+        <v>1</v>
       </c>
       <c r="P17" s="31" t="s">
         <v>39</v>
@@ -4265,9 +4317,9 @@
       <c r="A3" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="39" t="str">
+      <c r="B3" s="39">
         <f>'Week 2 Review'!E$17</f>
-        <v>NA</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <f>'Week 2 Review'!Y$7</f>
@@ -4280,9 +4332,9 @@
       <c r="E3" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="39" t="str">
+      <c r="F3" s="39">
         <f>'Week 2 Review'!O$17</f>
-        <v>NA</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <f>'Week 2 Review'!Y$12</f>
@@ -4395,9 +4447,9 @@
       <c r="A8" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="39" t="str">
+      <c r="B8" s="39">
         <f>'Week 2 Review'!G$17</f>
-        <v>NA</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <f>'Week 2 Review'!Y$8</f>
@@ -4525,9 +4577,9 @@
       <c r="A13" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="39" t="str">
+      <c r="B13" s="39">
         <f>'Week 2 Review'!I$17</f>
-        <v>NA</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <f>'Week 2 Review'!Y$9</f>
@@ -4656,9 +4708,9 @@
       <c r="A18" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="39" t="str">
+      <c r="B18" s="39">
         <f>'Week 2 Review'!K$17</f>
-        <v>NA</v>
+        <v>1</v>
       </c>
       <c r="C18">
         <f>'Week 2 Review'!Y$10</f>
@@ -4788,9 +4840,9 @@
       <c r="A23" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="39" t="str">
+      <c r="B23" s="39">
         <f>'Week 2 Review'!M$17</f>
-        <v>NA</v>
+        <v>1</v>
       </c>
       <c r="C23">
         <f>'Week 2 Review'!Y$11</f>

</xml_diff>

<commit_message>
[Add] peer review glyn
</commit_message>
<xml_diff>
--- a/Design Docs/PeerReview.xlsx
+++ b/Design Docs/PeerReview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project-startup\Design Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Y2\Block 3\Project startup\Design Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDB8D60-05F9-420E-92FA-0E06EC3D55B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA1DC5F-428C-4D07-AFC5-2207E8246F09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 2 Review" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,14 @@
     <sheet name="Progress Overview" sheetId="4" r:id="rId4"/>
     <sheet name="Data" sheetId="5" state="hidden" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="58">
   <si>
     <t>PEER1</t>
   </si>
@@ -206,6 +208,24 @@
 Punctuality Improved compared previous Projects.
 Improvement(s):
 </t>
+  </si>
+  <si>
+    <t>Strength(s):
+You feel very responsible over your tasks and take them very seriously. Urging our team to start using HacknPlan more seriously has really increased the profesionality of our planning and scheduling.
+Improvement(s):
+Late hours might sometimes be necessary but should not be so. Workload could be more shared between people, or better planned for.</t>
+  </si>
+  <si>
+    <t>Strength(s):
+You feel responsible for your tasks and you work hard to complete them, you make sure you're in office in time and you're never missing without good reason. You're very reliable.
+Improvement(s):
+Workload estimation seems to be something you were struggling with. try to estimate how much time it would take you and add 30%.</t>
+  </si>
+  <si>
+    <t>Strength(s):
+You are reliable and fast to work, you deliver your deliverable with a high quality in a timely manner. You discuss your work to find feedback during development.
+Improvement(s):
+After you're done with your work I didn't know what you all put into the sound moodboard untill the presentation, which also didn't allow people to give any more feedback</t>
   </si>
 </sst>
 </file>
@@ -1130,8 +1150,8 @@
   </sheetPr>
   <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1668,15 +1688,19 @@
         <v>47</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="24"/>
+        <v>55</v>
+      </c>
+      <c r="E11" s="24">
+        <v>8</v>
+      </c>
       <c r="F11" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="24"/>
+        <v>56</v>
+      </c>
+      <c r="G11" s="24">
+        <v>8</v>
+      </c>
       <c r="H11" s="40" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="I11" s="24"/>
       <c r="J11" s="22" t="s">
@@ -1978,16 +2002,16 @@
       <c r="D17" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="33" t="str">
+      <c r="E17" s="33">
         <f>IF(COUNTA(E7:E16)&gt;0,COUNT(E7:E16)/COUNTA(E7:E16),"NA")</f>
-        <v>NA</v>
+        <v>1</v>
       </c>
       <c r="F17" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="33" t="str">
+      <c r="G17" s="33">
         <f>IF(COUNTA(G7:G16)&gt;0,COUNT(G7:G16)/COUNTA(G7:G16),"NA")</f>
-        <v>NA</v>
+        <v>1</v>
       </c>
       <c r="H17" s="31" t="s">
         <v>39</v>
@@ -4265,9 +4289,9 @@
       <c r="A3" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="39" t="str">
+      <c r="B3" s="39">
         <f>'Week 2 Review'!E$17</f>
-        <v>NA</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <f>'Week 2 Review'!Y$7</f>
@@ -4395,9 +4419,9 @@
       <c r="A8" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="39" t="str">
+      <c r="B8" s="39">
         <f>'Week 2 Review'!G$17</f>
-        <v>NA</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <f>'Week 2 Review'!Y$8</f>

</xml_diff>